<commit_message>
Parseo de fórmulas funcionando
</commit_message>
<xml_diff>
--- a/tests/files/testing.xlsx
+++ b/tests/files/testing.xlsx
@@ -2,15 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Testing" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -19,7 +20,7 @@
   <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
@@ -50,9 +51,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -125,7 +126,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -135,44 +136,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -199,32 +200,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -251,24 +234,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -280,162 +245,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr"/>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -451,28 +420,28 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0"/>
+    <outlinePr summaryBelow="0" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="35" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="5"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
@@ -512,19 +481,19 @@
         </is>
       </c>
       <c r="B2">
-        <f>SUM(B4,B17)</f>
+        <f>SUM(B3,B16)</f>
         <v/>
       </c>
       <c r="C2">
-        <f>SUM(C4,C17)</f>
+        <f>SUM(C3,C16)</f>
         <v/>
       </c>
       <c r="D2">
-        <f>SUM(D4,D17)</f>
+        <f>SUM(D3,D16)</f>
         <v/>
       </c>
       <c r="E2">
-        <f>SUM(E4,E17)</f>
+        <f>SUM(E3,E16)</f>
         <v/>
       </c>
     </row>
@@ -535,19 +504,19 @@
         </is>
       </c>
       <c r="B3">
-        <f>SUM(B5,B11,B14)</f>
+        <f>SUM(B4,B10,B13)</f>
         <v/>
       </c>
       <c r="C3">
-        <f>SUM(C5,C11,C14)</f>
+        <f>SUM(C4,C10,C13)</f>
         <v/>
       </c>
       <c r="D3">
-        <f>SUM(D5,D11,D14)</f>
+        <f>SUM(D4,D10,D13)</f>
         <v/>
       </c>
       <c r="E3">
-        <f>SUM(E5,E11,E14)</f>
+        <f>SUM(E4,E10,E13)</f>
         <v/>
       </c>
     </row>
@@ -558,19 +527,19 @@
         </is>
       </c>
       <c r="B4">
-        <f>SUM(B6:B7:B8:B9:B10)</f>
+        <f>SUM(B5:B9)</f>
         <v/>
       </c>
       <c r="C4">
-        <f>SUM(C6:C7:C8:C9:C10)</f>
+        <f>SUM(C5:C9)</f>
         <v/>
       </c>
       <c r="D4">
-        <f>SUM(D6:D7:D8:D9:D10)</f>
+        <f>SUM(D5:D9)</f>
         <v/>
       </c>
       <c r="E4">
-        <f>SUM(E6:E7:E8:E9:E10)</f>
+        <f>SUM(E5:E9)</f>
         <v/>
       </c>
     </row>
@@ -676,19 +645,19 @@
         </is>
       </c>
       <c r="B10">
-        <f>SUM(B12:B13)</f>
+        <f>SUM(B11:B12)</f>
         <v/>
       </c>
       <c r="C10">
-        <f>SUM(C12:C13)</f>
+        <f>SUM(C11:C12)</f>
         <v/>
       </c>
       <c r="D10">
-        <f>SUM(D12:D13)</f>
+        <f>SUM(D11:D12)</f>
         <v/>
       </c>
       <c r="E10">
-        <f>SUM(E12:E13)</f>
+        <f>SUM(E11:E12)</f>
         <v/>
       </c>
     </row>
@@ -737,19 +706,19 @@
         </is>
       </c>
       <c r="B13">
-        <f>SUM(B15:B16)</f>
+        <f>SUM(B14:B15)</f>
         <v/>
       </c>
       <c r="C13">
-        <f>SUM(C15:C16)</f>
+        <f>SUM(C14:C15)</f>
         <v/>
       </c>
       <c r="D13">
-        <f>SUM(D15:D16)</f>
+        <f>SUM(D14:D15)</f>
         <v/>
       </c>
       <c r="E13">
-        <f>SUM(E15:E16)</f>
+        <f>SUM(E14:E15)</f>
         <v/>
       </c>
     </row>
@@ -798,19 +767,19 @@
         </is>
       </c>
       <c r="B16">
-        <f>SUM(B18,B20,B24,B26,B28)</f>
+        <f>SUM(B17,B19,B23,B25,B27)</f>
         <v/>
       </c>
       <c r="C16">
-        <f>SUM(C18,C20,C24,C26,C28)</f>
+        <f>SUM(C17,C19,C23,C25,C27)</f>
         <v/>
       </c>
       <c r="D16">
-        <f>SUM(D18,D20,D24,D26,D28)</f>
+        <f>SUM(D17,D19,D23,D25,D27)</f>
         <v/>
       </c>
       <c r="E16">
-        <f>SUM(E18,E20,E24,E26,E28)</f>
+        <f>SUM(E17,E19,E23,E25,E27)</f>
         <v/>
       </c>
     </row>
@@ -821,19 +790,19 @@
         </is>
       </c>
       <c r="B17">
-        <f>SUM(B19)</f>
+        <f>SUM(B18)</f>
         <v/>
       </c>
       <c r="C17">
-        <f>SUM(C19)</f>
+        <f>SUM(C18)</f>
         <v/>
       </c>
       <c r="D17">
-        <f>SUM(D19)</f>
+        <f>SUM(D18)</f>
         <v/>
       </c>
       <c r="E17">
-        <f>SUM(E19)</f>
+        <f>SUM(E18)</f>
         <v/>
       </c>
     </row>
@@ -863,19 +832,19 @@
         </is>
       </c>
       <c r="B19">
-        <f>SUM(B21:B22:B23)</f>
+        <f>SUM(B20:B22)</f>
         <v/>
       </c>
       <c r="C19">
-        <f>SUM(C21:C22:C23)</f>
+        <f>SUM(C20:C22)</f>
         <v/>
       </c>
       <c r="D19">
-        <f>SUM(D21:D22:D23)</f>
+        <f>SUM(D20:D22)</f>
         <v/>
       </c>
       <c r="E19">
-        <f>SUM(E21:E22:E23)</f>
+        <f>SUM(E20:E22)</f>
         <v/>
       </c>
     </row>
@@ -943,19 +912,19 @@
         </is>
       </c>
       <c r="B23">
-        <f>SUM(B25)</f>
+        <f>SUM(B24)</f>
         <v/>
       </c>
       <c r="C23">
-        <f>SUM(C25)</f>
+        <f>SUM(C24)</f>
         <v/>
       </c>
       <c r="D23">
-        <f>SUM(D25)</f>
+        <f>SUM(D24)</f>
         <v/>
       </c>
       <c r="E23">
-        <f>SUM(E25)</f>
+        <f>SUM(E24)</f>
         <v/>
       </c>
     </row>
@@ -985,19 +954,19 @@
         </is>
       </c>
       <c r="B25">
-        <f>SUM(B27)</f>
+        <f>SUM(B26)</f>
         <v/>
       </c>
       <c r="C25">
-        <f>SUM(C27)</f>
+        <f>SUM(C26)</f>
         <v/>
       </c>
       <c r="D25">
-        <f>SUM(D27)</f>
+        <f>SUM(D26)</f>
         <v/>
       </c>
       <c r="E25">
-        <f>SUM(E27)</f>
+        <f>SUM(E26)</f>
         <v/>
       </c>
     </row>
@@ -1027,19 +996,19 @@
         </is>
       </c>
       <c r="B27">
-        <f>SUM(B29)</f>
+        <f>SUM(B28)</f>
         <v/>
       </c>
       <c r="C27">
-        <f>SUM(C29)</f>
+        <f>SUM(C28)</f>
         <v/>
       </c>
       <c r="D27">
-        <f>SUM(D29)</f>
+        <f>SUM(D28)</f>
         <v/>
       </c>
       <c r="E27">
-        <f>SUM(E29)</f>
+        <f>SUM(E28)</f>
         <v/>
       </c>
     </row>
@@ -1069,19 +1038,19 @@
         </is>
       </c>
       <c r="B29">
-        <f>SUM(B31)</f>
+        <f>SUM(B30)</f>
         <v/>
       </c>
       <c r="C29">
-        <f>SUM(C31)</f>
+        <f>SUM(C30)</f>
         <v/>
       </c>
       <c r="D29">
-        <f>SUM(D31)</f>
+        <f>SUM(D30)</f>
         <v/>
       </c>
       <c r="E29">
-        <f>SUM(E31)</f>
+        <f>SUM(E30)</f>
         <v/>
       </c>
     </row>
@@ -1092,19 +1061,19 @@
         </is>
       </c>
       <c r="B30">
-        <f>SUM()</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="C30">
-        <f>SUM()</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="D30">
-        <f>SUM()</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="E30">
-        <f>SUM()</f>
+        <f>0</f>
         <v/>
       </c>
     </row>
@@ -1115,19 +1084,19 @@
         </is>
       </c>
       <c r="B31">
-        <f>SUM()</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="C31">
-        <f>SUM()</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="D31">
-        <f>SUM()</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="E31">
-        <f>SUM()</f>
+        <f>0</f>
         <v/>
       </c>
     </row>
@@ -1138,19 +1107,19 @@
         </is>
       </c>
       <c r="B32">
-        <f>B3 - B30</f>
+        <f>B2-B29</f>
         <v/>
       </c>
       <c r="C32">
-        <f>C3 - C30</f>
+        <f>C2-C29</f>
         <v/>
       </c>
       <c r="D32">
-        <f>D3 - D30</f>
+        <f>D2-D29</f>
         <v/>
       </c>
       <c r="E32">
-        <f>E3 - E30</f>
+        <f>E2-E29</f>
         <v/>
       </c>
     </row>

</xml_diff>